<commit_message>
Updated Texas State Data
</commit_message>
<xml_diff>
--- a/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
+++ b/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\CMartStudios\collincountycoviddashboard\Services\StateOfTexas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92963A40-A450-456B-BB1A-DA832BE68971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CADD9A4-E41C-48AE-B2CD-2222668A4CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-19 Hospitalizations" sheetId="4" r:id="rId1"/>
@@ -382,9 +382,6 @@
     <t>2020-08-07</t>
   </si>
   <si>
-    <t>2020-08-08</t>
-  </si>
-  <si>
     <t>2020-08-09</t>
   </si>
   <si>
@@ -406,9 +403,6 @@
     <t>2020-08-15</t>
   </si>
   <si>
-    <t>2020-08-16</t>
-  </si>
-  <si>
     <t>2020-08-17</t>
   </si>
   <si>
@@ -746,6 +740,12 @@
   </si>
   <si>
     <t>2020-12-07</t>
+  </si>
+  <si>
+    <t>2020-12-08</t>
+  </si>
+  <si>
+    <t>2020-12-09</t>
   </si>
   <si>
     <t>E.</t>
@@ -758,7 +758,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -770,12 +770,6 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -814,7 +808,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1131,9 +1125,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:IH2"/>
+  <dimension ref="A1:IJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="DE1" workbookViewId="0">
       <selection activeCell="DY2" sqref="DY2"/>
     </sheetView>
   </sheetViews>
@@ -1141,12 +1135,11 @@
   <cols>
     <col min="120" max="120" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="129" max="129" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:242" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:244" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1507,374 +1500,380 @@
       <c r="DP1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DQ1" s="2">
+        <v>44050</v>
+      </c>
+      <c r="DR1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DS1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DW1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="2">
+        <v>44059</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="EA1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EC1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" s="1" t="s">
+      <c r="EE1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" s="1" t="s">
+      <c r="EF1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" s="1" t="s">
+      <c r="EG1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="EI1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EK1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EM1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EN1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="EO1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" s="1" t="s">
+      <c r="EQ1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" s="1" t="s">
+      <c r="ER1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" s="1" t="s">
+      <c r="ES1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" s="1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="EV1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="EW1" s="1" t="s">
+      <c r="EY1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="EX1" s="1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="EY1" s="1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="EZ1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="FA1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="FB1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="FD1" s="1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="FE1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="FF1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="FG1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="FH1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="FJ1" s="1" t="s">
+      <c r="FL1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="FK1" s="1" t="s">
+      <c r="FM1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FN1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FP1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="FO1" s="1" t="s">
+      <c r="FQ1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="FP1" s="1" t="s">
+      <c r="FR1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="FQ1" s="1" t="s">
+      <c r="FS1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="FR1" s="1" t="s">
+      <c r="FT1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="FS1" s="1" t="s">
+      <c r="FU1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="FT1" s="1" t="s">
+      <c r="FV1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="FU1" s="1" t="s">
+      <c r="FW1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="FV1" s="1" t="s">
+      <c r="FX1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="FW1" s="1" t="s">
+      <c r="FY1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="FX1" s="1" t="s">
+      <c r="FZ1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="FY1" s="1" t="s">
+      <c r="GA1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="FZ1" s="1" t="s">
+      <c r="GB1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GC1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="GB1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="GC1" s="1" t="s">
+      <c r="GE1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="GD1" s="1" t="s">
+      <c r="GF1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="GE1" s="1" t="s">
+      <c r="GG1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="GF1" s="1" t="s">
+      <c r="GH1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="GG1" s="1" t="s">
+      <c r="GI1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="GH1" s="1" t="s">
+      <c r="GJ1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="GI1" s="1" t="s">
+      <c r="GK1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="GJ1" s="1" t="s">
+      <c r="GL1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="GK1" s="1" t="s">
+      <c r="GM1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="GL1" s="1" t="s">
+      <c r="GN1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="GM1" s="1" t="s">
+      <c r="GO1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="GN1" s="1" t="s">
+      <c r="GP1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="GO1" s="1" t="s">
+      <c r="GQ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="GP1" s="1" t="s">
+      <c r="GR1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="GQ1" s="1" t="s">
+      <c r="GS1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="GR1" s="1" t="s">
+      <c r="GT1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="GS1" s="1" t="s">
+      <c r="GU1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="GT1" s="1" t="s">
+      <c r="GV1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="GU1" s="1" t="s">
+      <c r="GW1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="GV1" s="1" t="s">
+      <c r="GX1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="GW1" s="1" t="s">
+      <c r="GY1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="GX1" s="1" t="s">
+      <c r="GZ1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="GY1" s="1" t="s">
+      <c r="HA1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="GZ1" s="1" t="s">
+      <c r="HB1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="HA1" s="1" t="s">
+      <c r="HC1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="HB1" s="1" t="s">
+      <c r="HD1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="HC1" s="1" t="s">
+      <c r="HE1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="HD1" s="1" t="s">
+      <c r="HF1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="HE1" s="1" t="s">
+      <c r="HG1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="HF1" s="1" t="s">
+      <c r="HH1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="HG1" s="1" t="s">
+      <c r="HI1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="HH1" s="1" t="s">
+      <c r="HJ1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="HI1" s="1" t="s">
+      <c r="HK1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="HJ1" s="1" t="s">
+      <c r="HL1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="HK1" s="1" t="s">
+      <c r="HM1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="HL1" s="1" t="s">
+      <c r="HN1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="HM1" s="1" t="s">
+      <c r="HO1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="HN1" s="1" t="s">
+      <c r="HP1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="HO1" s="1" t="s">
+      <c r="HQ1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="HP1" s="1" t="s">
+      <c r="HR1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="HQ1" s="1" t="s">
+      <c r="HS1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="HR1" s="1" t="s">
+      <c r="HT1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="HS1" s="1" t="s">
+      <c r="HU1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="HT1" s="1" t="s">
+      <c r="HV1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="HU1" s="1" t="s">
+      <c r="HW1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="HV1" s="1" t="s">
+      <c r="HX1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="HW1" s="1" t="s">
+      <c r="HY1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="HX1" s="1" t="s">
+      <c r="HZ1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="HY1" s="1" t="s">
+      <c r="IA1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="HZ1" s="1" t="s">
+      <c r="IB1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="IA1" s="1" t="s">
+      <c r="IC1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="IB1" s="1" t="s">
+      <c r="ID1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="IC1" s="1" t="s">
+      <c r="IE1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="ID1" s="1" t="s">
+      <c r="IF1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="IE1" s="1" t="s">
+      <c r="IG1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="IF1" s="1" t="s">
+      <c r="IH1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="IG1" s="1" t="s">
+      <c r="II1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="IH1" s="1" t="s">
+      <c r="IJ1" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:242" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:244" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>242</v>
       </c>
@@ -2600,10 +2599,15 @@
       </c>
       <c r="IH2">
         <v>2460</v>
+      </c>
+      <c r="II2">
+        <v>2563</v>
+      </c>
+      <c r="IJ2">
+        <v>2542</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Latest Hospitalization tile to show Covid % of capacity rather than hospitalization delta
</commit_message>
<xml_diff>
--- a/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
+++ b/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\CMartStudios\collincountycoviddashboard\Services\StateOfTexas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B678C2F-A392-4793-86B9-05298CBCD556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20275F40-D46A-498B-807C-1738841CBE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-19 Hospitalizations" sheetId="1" r:id="rId1"/>
+    <sheet name="GA-32 COVID % Capacity" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="246">
   <si>
     <t>TSA ID</t>
   </si>
@@ -755,6 +756,9 @@
   </si>
   <si>
     <t>Dallas/Ft. Worth</t>
+  </si>
+  <si>
+    <t>2020-08-08</t>
   </si>
 </sst>
 </file>
@@ -806,11 +810,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1130,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="EA1" sqref="EA1"/>
+    <sheetView tabSelected="1" topLeftCell="DE1" workbookViewId="0">
+      <selection activeCell="DX1" sqref="DX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1506,7 @@
       <c r="DP1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="2">
+      <c r="DQ1" s="3">
         <v>44051</v>
       </c>
       <c r="DR1" s="1" t="s">
@@ -1525,7 +1530,7 @@
       <c r="DX1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="DY1" s="2">
+      <c r="DY1" s="3">
         <v>44059</v>
       </c>
       <c r="DZ1" s="1" t="s">
@@ -2616,5 +2621,1499 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:IK2"/>
+  <sheetViews>
+    <sheetView topLeftCell="HN1" workbookViewId="0">
+      <selection activeCell="IK2" sqref="IK2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="129" max="129" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:245" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DY1" s="3">
+        <v>44059</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EP1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="ES1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="ET1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="EU1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="EV1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="EW1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EX1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="EY1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="FA1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="FB1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="FC1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="FD1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="FE1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="FF1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="FG1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="FH1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="FI1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="FJ1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="FK1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="FL1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="FM1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="FN1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="FO1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="FP1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="FQ1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="FR1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="FS1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="FT1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="FU1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="FV1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="FW1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="FX1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="FY1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="FZ1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="GA1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="GB1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="GC1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="GD1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="GE1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="GF1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="GG1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="GH1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="GI1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="GK1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="GL1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="GM1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="GN1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="GP1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="GQ1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="GR1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="GS1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="GY1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="GZ1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="HA1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="HB1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="HC1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="HD1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="HE1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="HF1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="HG1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="HH1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="HI1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="HJ1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="HK1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="HL1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="HM1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="HN1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="HO1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="HP1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="HQ1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="HR1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="HS1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="HT1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="HU1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="HV1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="HW1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="HX1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="HY1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="HZ1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="IA1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="IB1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="IC1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="ID1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="IE1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="IF1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="IG1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="IH1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="II1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="IJ1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="IK1" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:245" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.9657611316508601E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.7153697366463322E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.6765212399540758E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.9558920342330479E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.2487730697449368E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.2175206164661352E-2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.0648048693161477E-2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3.0923437833226701E-2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>3.1543314356054779E-2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>3.1389499043435132E-2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>3.4020397974466869E-2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3.4965507912890575E-2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>3.6433492315845258E-2</v>
+      </c>
+      <c r="P2" s="2">
+        <v>3.5864252770702827E-2</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>3.3719102728961281E-2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>3.5293271995399653E-2</v>
+      </c>
+      <c r="S2" s="2">
+        <v>3.8801996672212978E-2</v>
+      </c>
+      <c r="T2" s="2">
+        <v>4.0252981092298572E-2</v>
+      </c>
+      <c r="U2" s="2">
+        <v>3.9930675909878685E-2</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4.2085759661196404E-2</v>
+      </c>
+      <c r="W2" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X2" s="2">
+        <v>3.9146170322771255E-2</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>3.956196498804658E-2</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>4.8074179743223963E-2</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>4.5813372916807232E-2</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>4.7000140508641285E-2</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>4.5256744995648392E-2</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>4.4305091677458934E-2</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>4.0587773735644483E-2</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>4.0464193006565889E-2</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>4.7793599323276467E-2</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>4.3181818181818182E-2</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>4.5560268162539337E-2</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>4.539082838261798E-2</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>4.7322970639032819E-2</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>4.1453505868191395E-2</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>4.4507042253521124E-2</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>4.6291651737728416E-2</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>4.2665609933293706E-2</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>4.0406761398073941E-2</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>3.8513513513513516E-2</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>4.1777595740323574E-2</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>4.2666448284333795E-2</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>4.0293317205926819E-2</v>
+      </c>
+      <c r="AV2" s="2">
+        <v>4.2616308516026338E-2</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>4.313256403039685E-2</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>3.9373814041745732E-2</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>4.1616646658663464E-2</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>4.0476190476190478E-2</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>4.0630472854640984E-2</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>3.9925910681210125E-2</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>3.9745627980922099E-2</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>4.0520595733261777E-2</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>4.0473309130025545E-2</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>4.1333606613377059E-2</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>4.2471042471042469E-2</v>
+      </c>
+      <c r="BH2" s="2">
+        <v>4.6885773385428639E-2</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>4.7261009667024706E-2</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>4.7376043031515068E-2</v>
+      </c>
+      <c r="BK2" s="2">
+        <v>4.8300904357358183E-2</v>
+      </c>
+      <c r="BL2" s="2">
+        <v>4.8402447314751872E-2</v>
+      </c>
+      <c r="BM2" s="2">
+        <v>5.0255066868881842E-2</v>
+      </c>
+      <c r="BN2" s="2">
+        <v>5.1576337229897275E-2</v>
+      </c>
+      <c r="BO2" s="2">
+        <v>5.5954661558109832E-2</v>
+      </c>
+      <c r="BP2" s="2">
+        <v>5.3187791142320792E-2</v>
+      </c>
+      <c r="BQ2" s="2">
+        <v>5.8359942930905635E-2</v>
+      </c>
+      <c r="BR2" s="2">
+        <v>5.9571930289576566E-2</v>
+      </c>
+      <c r="BS2" s="2">
+        <v>6.0449735449735448E-2</v>
+      </c>
+      <c r="BT2" s="2">
+        <v>6.2487522459572772E-2</v>
+      </c>
+      <c r="BU2" s="2">
+        <v>6.5420560747663545E-2</v>
+      </c>
+      <c r="BV2" s="2">
+        <v>6.9705093833780166E-2</v>
+      </c>
+      <c r="BW2" s="2">
+        <v>7.5729798335918766E-2</v>
+      </c>
+      <c r="BX2" s="2">
+        <v>7.7217438841055072E-2</v>
+      </c>
+      <c r="BY2" s="2">
+        <v>7.6457534799273752E-2</v>
+      </c>
+      <c r="BZ2" s="2">
+        <v>7.9215896885069817E-2</v>
+      </c>
+      <c r="CA2" s="2">
+        <v>8.4478440398023422E-2</v>
+      </c>
+      <c r="CB2" s="2">
+        <v>8.7917451021404164E-2</v>
+      </c>
+      <c r="CC2" s="2">
+        <v>9.1750961675452339E-2</v>
+      </c>
+      <c r="CD2" s="2">
+        <v>9.8179221706533384E-2</v>
+      </c>
+      <c r="CE2" s="2">
+        <v>9.4425483503981791E-2</v>
+      </c>
+      <c r="CF2" s="2">
+        <v>0.10195198258858737</v>
+      </c>
+      <c r="CG2" s="2">
+        <v>0.10407055630936228</v>
+      </c>
+      <c r="CH2" s="2">
+        <v>0.10573934663996132</v>
+      </c>
+      <c r="CI2" s="2">
+        <v>0.11003099464637926</v>
+      </c>
+      <c r="CJ2" s="2">
+        <v>0.11874676716175275</v>
+      </c>
+      <c r="CK2" s="2">
+        <v>0.12417109961378707</v>
+      </c>
+      <c r="CL2" s="2">
+        <v>0.12721518987341773</v>
+      </c>
+      <c r="CM2" s="2">
+        <v>0.12627065901389944</v>
+      </c>
+      <c r="CN2" s="2">
+        <v>0.12915689250724438</v>
+      </c>
+      <c r="CO2" s="2">
+        <v>0.12441202535960189</v>
+      </c>
+      <c r="CP2" s="2">
+        <v>0.12703626734598109</v>
+      </c>
+      <c r="CQ2" s="2">
+        <v>0.13252413401476434</v>
+      </c>
+      <c r="CR2" s="2">
+        <v>0.13045024539440928</v>
+      </c>
+      <c r="CS2" s="2">
+        <v>0.12817144832353958</v>
+      </c>
+      <c r="CT2" s="2">
+        <v>0.12670171182100012</v>
+      </c>
+      <c r="CU2" s="2">
+        <v>0.12875075518560783</v>
+      </c>
+      <c r="CV2" s="2">
+        <v>0.12841604350781782</v>
+      </c>
+      <c r="CW2" s="2">
+        <v>0.13257549340958225</v>
+      </c>
+      <c r="CX2" s="2">
+        <v>0.13674112256586485</v>
+      </c>
+      <c r="CY2" s="2">
+        <v>0.13430523276287062</v>
+      </c>
+      <c r="CZ2" s="2">
+        <v>0.13700062748378999</v>
+      </c>
+      <c r="DA2" s="2">
+        <v>8.1793122147408373E-2</v>
+      </c>
+      <c r="DB2" s="2">
+        <v>0.13671875</v>
+      </c>
+      <c r="DC2" s="2">
+        <v>0.12792604741315045</v>
+      </c>
+      <c r="DD2" s="2">
+        <v>0.1415259172976121</v>
+      </c>
+      <c r="DE2" s="2">
+        <v>0.11662265362929126</v>
+      </c>
+      <c r="DF2" s="2">
+        <v>0.12722764605609793</v>
+      </c>
+      <c r="DG2" s="2">
+        <v>0.12926701177882813</v>
+      </c>
+      <c r="DH2" s="2">
+        <v>0.11138898276444745</v>
+      </c>
+      <c r="DI2" s="2">
+        <v>0.1183334579998504</v>
+      </c>
+      <c r="DJ2" s="2">
+        <v>0.11844305914550707</v>
+      </c>
+      <c r="DK2" s="2">
+        <v>0.11564160971905847</v>
+      </c>
+      <c r="DL2" s="2">
+        <v>0.12236974920413075</v>
+      </c>
+      <c r="DM2" s="2">
+        <v>0.11791660302428593</v>
+      </c>
+      <c r="DN2" s="2">
+        <v>0.10770559033023959</v>
+      </c>
+      <c r="DO2" s="2">
+        <v>0.1029097133076594</v>
+      </c>
+      <c r="DP2" s="2">
+        <v>9.871396269078575E-2</v>
+      </c>
+      <c r="DQ2" s="2">
+        <v>9.6863000796928209E-2</v>
+      </c>
+      <c r="DR2" s="2">
+        <v>9.6040682891391213E-2</v>
+      </c>
+      <c r="DS2" s="2">
+        <v>9.8441219381094985E-2</v>
+      </c>
+      <c r="DT2" s="2">
+        <v>9.1617210682492581E-2</v>
+      </c>
+      <c r="DU2" s="2">
+        <v>8.9472917880023303E-2</v>
+      </c>
+      <c r="DV2" s="2">
+        <v>8.7834870443566096E-2</v>
+      </c>
+      <c r="DW2" s="2">
+        <v>8.8184187662901828E-2</v>
+      </c>
+      <c r="DX2" s="2">
+        <v>8.9361702127659579E-2</v>
+      </c>
+      <c r="DY2" s="2">
+        <v>8.4202085004009622E-2</v>
+      </c>
+      <c r="DZ2" s="2">
+        <v>8.7521001985642277E-2</v>
+      </c>
+      <c r="EA2" s="2">
+        <v>8.6554621848739494E-2</v>
+      </c>
+      <c r="EB2" s="2">
+        <v>8.0152102594691327E-2</v>
+      </c>
+      <c r="EC2" s="2">
+        <v>7.8339645058290636E-2</v>
+      </c>
+      <c r="ED2" s="2">
+        <v>7.5844952186290976E-2</v>
+      </c>
+      <c r="EE2" s="2">
+        <v>7.5027829313543598E-2</v>
+      </c>
+      <c r="EF2" s="2">
+        <v>7.1905609973285836E-2</v>
+      </c>
+      <c r="EG2" s="2">
+        <v>7.3048623226883103E-2</v>
+      </c>
+      <c r="EH2" s="2">
+        <v>7.2435395458104929E-2</v>
+      </c>
+      <c r="EI2" s="2">
+        <v>7.0755433956528349E-2</v>
+      </c>
+      <c r="EJ2" s="2">
+        <v>6.7698259187620888E-2</v>
+      </c>
+      <c r="EK2" s="2">
+        <v>6.4431102650461272E-2</v>
+      </c>
+      <c r="EL2" s="2">
+        <v>6.4513772192591509E-2</v>
+      </c>
+      <c r="EM2" s="2">
+        <v>6.2855454612600642E-2</v>
+      </c>
+      <c r="EN2" s="2">
+        <v>6.0754496271384704E-2</v>
+      </c>
+      <c r="EO2" s="2">
+        <v>6.3898971566848151E-2</v>
+      </c>
+      <c r="EP2" s="2">
+        <v>6.1093484837305395E-2</v>
+      </c>
+      <c r="EQ2" s="2">
+        <v>5.8212209302325582E-2</v>
+      </c>
+      <c r="ER2" s="2">
+        <v>5.6153013352580293E-2</v>
+      </c>
+      <c r="ES2" s="2">
+        <v>6.5025850141993732E-2</v>
+      </c>
+      <c r="ET2" s="2">
+        <v>5.5914768552534903E-2</v>
+      </c>
+      <c r="EU2" s="2">
+        <v>5.1428137344272255E-2</v>
+      </c>
+      <c r="EV2" s="2">
+        <v>6.0331140848264915E-2</v>
+      </c>
+      <c r="EW2" s="2">
+        <v>5.8259029771799913E-2</v>
+      </c>
+      <c r="EX2" s="2">
+        <v>5.8248077066686582E-2</v>
+      </c>
+      <c r="EY2" s="2">
+        <v>5.4601048340128133E-2</v>
+      </c>
+      <c r="EZ2" s="2">
+        <v>5.5060187249219794E-2</v>
+      </c>
+      <c r="FA2" s="2">
+        <v>5.6709086849743247E-2</v>
+      </c>
+      <c r="FB2" s="2">
+        <v>5.7858634059051596E-2</v>
+      </c>
+      <c r="FC2" s="2">
+        <v>5.5726624108148708E-2</v>
+      </c>
+      <c r="FD2" s="2">
+        <v>5.2783386212864145E-2</v>
+      </c>
+      <c r="FE2" s="2">
+        <v>5.3703703703703705E-2</v>
+      </c>
+      <c r="FF2" s="2">
+        <v>5.3008998875140607E-2</v>
+      </c>
+      <c r="FG2" s="2">
+        <v>5.1326937889503536E-2</v>
+      </c>
+      <c r="FH2" s="2">
+        <v>5.328998515796169E-2</v>
+      </c>
+      <c r="FI2" s="2">
+        <v>5.3834543232947604E-2</v>
+      </c>
+      <c r="FJ2" s="2">
+        <v>5.5507621512798387E-2</v>
+      </c>
+      <c r="FK2" s="2">
+        <v>5.5575246331608423E-2</v>
+      </c>
+      <c r="FL2" s="2">
+        <v>5.5138020650417924E-2</v>
+      </c>
+      <c r="FM2" s="2">
+        <v>5.6429620306272292E-2</v>
+      </c>
+      <c r="FN2" s="2">
+        <v>5.6472571468708294E-2</v>
+      </c>
+      <c r="FO2" s="2">
+        <v>5.7207912338124375E-2</v>
+      </c>
+      <c r="FP2" s="2">
+        <v>5.7340266400740796E-2</v>
+      </c>
+      <c r="FQ2" s="2">
+        <v>6.0372977287569844E-2</v>
+      </c>
+      <c r="FR2" s="2">
+        <v>6.2938043173535185E-2</v>
+      </c>
+      <c r="FS2" s="2">
+        <v>5.4288666896314161E-2</v>
+      </c>
+      <c r="FT2" s="2">
+        <v>5.6721109820269254E-2</v>
+      </c>
+      <c r="FU2" s="2">
+        <v>5.7571700373476149E-2</v>
+      </c>
+      <c r="FV2" s="2">
+        <v>5.9160578713651338E-2</v>
+      </c>
+      <c r="FW2" s="2">
+        <v>6.4334836944464985E-2</v>
+      </c>
+      <c r="FX2" s="2">
+        <v>6.2689728203318043E-2</v>
+      </c>
+      <c r="FY2" s="2">
+        <v>6.4052195874842149E-2</v>
+      </c>
+      <c r="FZ2" s="2">
+        <v>6.2338369402477202E-2</v>
+      </c>
+      <c r="GA2" s="2">
+        <v>6.4068914462615256E-2</v>
+      </c>
+      <c r="GB2" s="2">
+        <v>6.6033898305084743E-2</v>
+      </c>
+      <c r="GC2" s="2">
+        <v>6.5638646288209604E-2</v>
+      </c>
+      <c r="GD2" s="2">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="GE2" s="2">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="GF2" s="2">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="GG2" s="2">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="GH2" s="2">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="GI2" s="2">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="GJ2" s="2">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="GK2" s="2">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="GL2" s="2">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="GM2" s="2">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="GN2" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="GO2" s="2">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="GP2" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="GQ2" s="2">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="GR2" s="2">
+        <v>9.9199999999999997E-2</v>
+      </c>
+      <c r="GS2" s="2">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="GT2" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="GU2" s="2">
+        <v>9.98E-2</v>
+      </c>
+      <c r="GV2" s="2">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="GW2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="GX2" s="2">
+        <v>0.1033</v>
+      </c>
+      <c r="GY2" s="2">
+        <v>0.1062</v>
+      </c>
+      <c r="GZ2" s="2">
+        <v>0.1085</v>
+      </c>
+      <c r="HA2" s="2">
+        <v>0.10730000000000001</v>
+      </c>
+      <c r="HB2" s="2">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="HC2" s="2">
+        <v>0.1009</v>
+      </c>
+      <c r="HD2" s="2">
+        <v>0.1028</v>
+      </c>
+      <c r="HE2" s="2">
+        <v>0.10290000000000001</v>
+      </c>
+      <c r="HF2" s="2">
+        <v>0.1089</v>
+      </c>
+      <c r="HG2" s="2">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="HH2" s="2">
+        <v>0.1197</v>
+      </c>
+      <c r="HI2" s="2">
+        <v>0.11749999999999999</v>
+      </c>
+      <c r="HJ2" s="2">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="HK2" s="2">
+        <v>0.1225</v>
+      </c>
+      <c r="HL2" s="2">
+        <v>0.1295</v>
+      </c>
+      <c r="HM2" s="2">
+        <v>0.13418910457107075</v>
+      </c>
+      <c r="HN2" s="2">
+        <v>0.1366</v>
+      </c>
+      <c r="HO2" s="2">
+        <v>0.1396</v>
+      </c>
+      <c r="HP2" s="2">
+        <v>0.1323</v>
+      </c>
+      <c r="HQ2" s="2">
+        <v>0.1358</v>
+      </c>
+      <c r="HR2" s="2">
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="HS2" s="2">
+        <v>0.1381</v>
+      </c>
+      <c r="HT2" s="2">
+        <v>0.1341</v>
+      </c>
+      <c r="HU2" s="2">
+        <v>0.14349999999999999</v>
+      </c>
+      <c r="HV2" s="2">
+        <v>0.14949999999999999</v>
+      </c>
+      <c r="HW2" s="2">
+        <v>0.1487</v>
+      </c>
+      <c r="HX2" s="2">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="HY2" s="2">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="HZ2" s="2">
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="IA2" s="2">
+        <v>0.1613</v>
+      </c>
+      <c r="IB2" s="2">
+        <v>0.1643</v>
+      </c>
+      <c r="IC2" s="2">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="ID2" s="2">
+        <v>0.15559999999999999</v>
+      </c>
+      <c r="IE2" s="2">
+        <v>0.1515</v>
+      </c>
+      <c r="IF2" s="2">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="IG2" s="2">
+        <v>0.1482</v>
+      </c>
+      <c r="IH2" s="2">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="II2" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="IJ2" s="2">
+        <v>0.1588</v>
+      </c>
+      <c r="IK2" s="2">
+        <v>0.15770000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up Seven Day Avg View
</commit_message>
<xml_diff>
--- a/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
+++ b/Services/StateOfTexas/Data/CombinedHospitalDataoverTimebyTSARegion.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\CMartStudios\collincountycoviddashboard\Services\StateOfTexas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA24FFB-B718-469F-BC51-16FBB47750F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAED931A-677F-4B88-B679-D96A01425CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-19 Hospitalizations" sheetId="1" r:id="rId1"/>
+    <sheet name="GA-32 COVID % Capacity" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="250">
   <si>
     <t>TSA ID</t>
   </si>
@@ -767,13 +768,16 @@
   </si>
   <si>
     <t>2020-12-12</t>
+  </si>
+  <si>
+    <t>2020-08-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -785,6 +789,13 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -815,10 +826,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,9 +839,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1143,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HL1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="IM2" sqref="IM2"/>
     </sheetView>
   </sheetViews>
@@ -2638,4 +2656,1505 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D29E0D1-F4C8-456B-B184-BCA63A3106C2}">
+  <dimension ref="A1:IM2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:IM2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:247" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="DR1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="DS1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="DT1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="ED1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="EE1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="EF1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="EG1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="EH1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="EJ1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="EK1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="EL1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EM1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="EN1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="EO1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="EP1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="EQ1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="ER1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="ES1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="ET1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="EU1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="EV1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="EW1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="EX1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="EY1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="EZ1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="FA1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="FB1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="FC1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="FD1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="FE1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="FF1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="FG1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="FH1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="FI1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="FJ1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="FK1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="FL1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="FM1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="FN1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="FO1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="FP1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="FQ1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="FR1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="FS1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="FT1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="FU1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="FV1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="FW1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="FX1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="FY1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="FZ1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="GA1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="GB1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="GC1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="GD1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="GE1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="GF1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="GG1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="GH1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="GI1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="GJ1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="GK1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="GL1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="GM1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="GN1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="GO1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="GP1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="GQ1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="GR1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="GS1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="GT1" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="GU1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="GV1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="GW1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="GX1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="GY1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="GZ1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="HA1" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="HB1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="HC1" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="HD1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="HE1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="HF1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="HG1" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="HH1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="HI1" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="HJ1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="HK1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="HL1" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="HM1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="HN1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="HO1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="HP1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="HQ1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="HR1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="HS1" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="HT1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="HU1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="HV1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="HW1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="HX1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="HY1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="HZ1" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="IA1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="IB1" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="IC1" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="ID1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="IE1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="IF1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="IG1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="IH1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="II1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="IJ1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="IK1" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="IL1" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="IM1" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:247" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.9657611316508601E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.7153697366463322E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2.6765212399540758E-2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2.9558920342330479E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3.2487730697449368E-2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3.2175206164661352E-2</v>
+      </c>
+      <c r="I2" s="6">
+        <v>3.0648048693161477E-2</v>
+      </c>
+      <c r="J2" s="6">
+        <v>3.0923437833226701E-2</v>
+      </c>
+      <c r="K2" s="6">
+        <v>3.1543314356054779E-2</v>
+      </c>
+      <c r="L2" s="6">
+        <v>3.1389499043435132E-2</v>
+      </c>
+      <c r="M2" s="6">
+        <v>3.4020397974466869E-2</v>
+      </c>
+      <c r="N2" s="6">
+        <v>3.4965507912890575E-2</v>
+      </c>
+      <c r="O2" s="6">
+        <v>3.6433492315845258E-2</v>
+      </c>
+      <c r="P2" s="6">
+        <v>3.5864252770702827E-2</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>3.3719102728961281E-2</v>
+      </c>
+      <c r="R2" s="6">
+        <v>3.5293271995399653E-2</v>
+      </c>
+      <c r="S2" s="6">
+        <v>3.8801996672212978E-2</v>
+      </c>
+      <c r="T2" s="6">
+        <v>4.0252981092298572E-2</v>
+      </c>
+      <c r="U2" s="6">
+        <v>3.9930675909878685E-2</v>
+      </c>
+      <c r="V2" s="6">
+        <v>4.2085759661196404E-2</v>
+      </c>
+      <c r="W2" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X2" s="6">
+        <v>3.9146170322771255E-2</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>3.956196498804658E-2</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>4.8074179743223963E-2</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>4.5813372916807232E-2</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>4.7000140508641285E-2</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>4.5256744995648392E-2</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>4.4305091677458934E-2</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>4.0587773735644483E-2</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>4.0464193006565889E-2</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>4.7793599323276467E-2</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>4.3181818181818182E-2</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>4.5560268162539337E-2</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>4.539082838261798E-2</v>
+      </c>
+      <c r="AK2" s="6">
+        <v>4.7322970639032819E-2</v>
+      </c>
+      <c r="AL2" s="6">
+        <v>4.1453505868191395E-2</v>
+      </c>
+      <c r="AM2" s="6">
+        <v>4.4507042253521124E-2</v>
+      </c>
+      <c r="AN2" s="6">
+        <v>4.6291651737728416E-2</v>
+      </c>
+      <c r="AO2" s="6">
+        <v>4.2665609933293706E-2</v>
+      </c>
+      <c r="AP2" s="6">
+        <v>4.0406761398073941E-2</v>
+      </c>
+      <c r="AQ2" s="6">
+        <v>3.8513513513513516E-2</v>
+      </c>
+      <c r="AR2" s="6">
+        <v>4.1777595740323574E-2</v>
+      </c>
+      <c r="AS2" s="6">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="AT2" s="6">
+        <v>4.2666448284333795E-2</v>
+      </c>
+      <c r="AU2" s="6">
+        <v>4.0293317205926819E-2</v>
+      </c>
+      <c r="AV2" s="6">
+        <v>4.2616308516026338E-2</v>
+      </c>
+      <c r="AW2" s="6">
+        <v>4.313256403039685E-2</v>
+      </c>
+      <c r="AX2" s="6">
+        <v>3.9373814041745732E-2</v>
+      </c>
+      <c r="AY2" s="6">
+        <v>4.1616646658663464E-2</v>
+      </c>
+      <c r="AZ2" s="6">
+        <v>4.0476190476190478E-2</v>
+      </c>
+      <c r="BA2" s="6">
+        <v>4.0630472854640984E-2</v>
+      </c>
+      <c r="BB2" s="6">
+        <v>3.9925910681210125E-2</v>
+      </c>
+      <c r="BC2" s="6">
+        <v>3.9745627980922099E-2</v>
+      </c>
+      <c r="BD2" s="6">
+        <v>4.0520595733261777E-2</v>
+      </c>
+      <c r="BE2" s="6">
+        <v>4.0473309130025545E-2</v>
+      </c>
+      <c r="BF2" s="6">
+        <v>4.1333606613377059E-2</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>4.2471042471042469E-2</v>
+      </c>
+      <c r="BH2" s="6">
+        <v>4.6885773385428639E-2</v>
+      </c>
+      <c r="BI2" s="6">
+        <v>4.7261009667024706E-2</v>
+      </c>
+      <c r="BJ2" s="6">
+        <v>4.7376043031515068E-2</v>
+      </c>
+      <c r="BK2" s="6">
+        <v>4.8300904357358183E-2</v>
+      </c>
+      <c r="BL2" s="6">
+        <v>4.8402447314751872E-2</v>
+      </c>
+      <c r="BM2" s="6">
+        <v>5.0255066868881842E-2</v>
+      </c>
+      <c r="BN2" s="6">
+        <v>5.1576337229897275E-2</v>
+      </c>
+      <c r="BO2" s="6">
+        <v>5.5954661558109832E-2</v>
+      </c>
+      <c r="BP2" s="6">
+        <v>5.3187791142320792E-2</v>
+      </c>
+      <c r="BQ2" s="6">
+        <v>5.8359942930905635E-2</v>
+      </c>
+      <c r="BR2" s="6">
+        <v>5.9571930289576566E-2</v>
+      </c>
+      <c r="BS2" s="6">
+        <v>6.0449735449735448E-2</v>
+      </c>
+      <c r="BT2" s="6">
+        <v>6.2487522459572772E-2</v>
+      </c>
+      <c r="BU2" s="6">
+        <v>6.5420560747663545E-2</v>
+      </c>
+      <c r="BV2" s="6">
+        <v>6.9705093833780166E-2</v>
+      </c>
+      <c r="BW2" s="6">
+        <v>7.5729798335918766E-2</v>
+      </c>
+      <c r="BX2" s="6">
+        <v>7.7217438841055072E-2</v>
+      </c>
+      <c r="BY2" s="6">
+        <v>7.6457534799273752E-2</v>
+      </c>
+      <c r="BZ2" s="6">
+        <v>7.9215896885069817E-2</v>
+      </c>
+      <c r="CA2" s="6">
+        <v>8.4478440398023422E-2</v>
+      </c>
+      <c r="CB2" s="6">
+        <v>8.7917451021404164E-2</v>
+      </c>
+      <c r="CC2" s="6">
+        <v>9.1750961675452339E-2</v>
+      </c>
+      <c r="CD2" s="6">
+        <v>9.8179221706533384E-2</v>
+      </c>
+      <c r="CE2" s="6">
+        <v>9.4425483503981791E-2</v>
+      </c>
+      <c r="CF2" s="6">
+        <v>0.10195198258858737</v>
+      </c>
+      <c r="CG2" s="6">
+        <v>0.10407055630936228</v>
+      </c>
+      <c r="CH2" s="6">
+        <v>0.10573934663996132</v>
+      </c>
+      <c r="CI2" s="6">
+        <v>0.11003099464637926</v>
+      </c>
+      <c r="CJ2" s="6">
+        <v>0.11874676716175275</v>
+      </c>
+      <c r="CK2" s="6">
+        <v>0.12417109961378707</v>
+      </c>
+      <c r="CL2" s="6">
+        <v>0.12721518987341773</v>
+      </c>
+      <c r="CM2" s="6">
+        <v>0.12627065901389944</v>
+      </c>
+      <c r="CN2" s="6">
+        <v>0.12915689250724438</v>
+      </c>
+      <c r="CO2" s="6">
+        <v>0.12441202535960189</v>
+      </c>
+      <c r="CP2" s="6">
+        <v>0.12703626734598109</v>
+      </c>
+      <c r="CQ2" s="6">
+        <v>0.13252413401476434</v>
+      </c>
+      <c r="CR2" s="6">
+        <v>0.13045024539440928</v>
+      </c>
+      <c r="CS2" s="6">
+        <v>0.12817144832353958</v>
+      </c>
+      <c r="CT2" s="6">
+        <v>0.12670171182100012</v>
+      </c>
+      <c r="CU2" s="6">
+        <v>0.12875075518560783</v>
+      </c>
+      <c r="CV2" s="6">
+        <v>0.12841604350781782</v>
+      </c>
+      <c r="CW2" s="6">
+        <v>0.13257549340958225</v>
+      </c>
+      <c r="CX2" s="6">
+        <v>0.13674112256586485</v>
+      </c>
+      <c r="CY2" s="6">
+        <v>0.13430523276287062</v>
+      </c>
+      <c r="CZ2" s="6">
+        <v>0.13700062748378999</v>
+      </c>
+      <c r="DA2" s="6">
+        <v>8.1793122147408373E-2</v>
+      </c>
+      <c r="DB2" s="6">
+        <v>0.13671875</v>
+      </c>
+      <c r="DC2" s="6">
+        <v>0.12792604741315045</v>
+      </c>
+      <c r="DD2" s="6">
+        <v>0.1415259172976121</v>
+      </c>
+      <c r="DE2" s="6">
+        <v>0.11662265362929126</v>
+      </c>
+      <c r="DF2" s="6">
+        <v>0.12722764605609793</v>
+      </c>
+      <c r="DG2" s="6">
+        <v>0.12926701177882813</v>
+      </c>
+      <c r="DH2" s="6">
+        <v>0.11138898276444745</v>
+      </c>
+      <c r="DI2" s="6">
+        <v>0.1183334579998504</v>
+      </c>
+      <c r="DJ2" s="6">
+        <v>0.11844305914550707</v>
+      </c>
+      <c r="DK2" s="6">
+        <v>0.11564160971905847</v>
+      </c>
+      <c r="DL2" s="6">
+        <v>0.12236974920413075</v>
+      </c>
+      <c r="DM2" s="6">
+        <v>0.11791660302428593</v>
+      </c>
+      <c r="DN2" s="6">
+        <v>0.10770559033023959</v>
+      </c>
+      <c r="DO2" s="6">
+        <v>0.1029097133076594</v>
+      </c>
+      <c r="DP2" s="6">
+        <v>9.871396269078575E-2</v>
+      </c>
+      <c r="DQ2" s="6">
+        <v>9.6863000796928209E-2</v>
+      </c>
+      <c r="DR2" s="6">
+        <v>9.6040682891391213E-2</v>
+      </c>
+      <c r="DS2" s="6">
+        <v>9.8441219381094985E-2</v>
+      </c>
+      <c r="DT2" s="6">
+        <v>9.1617210682492581E-2</v>
+      </c>
+      <c r="DU2" s="6">
+        <v>8.9472917880023303E-2</v>
+      </c>
+      <c r="DV2" s="6">
+        <v>8.7834870443566096E-2</v>
+      </c>
+      <c r="DW2" s="6">
+        <v>8.8184187662901828E-2</v>
+      </c>
+      <c r="DX2" s="6">
+        <v>8.9361702127659579E-2</v>
+      </c>
+      <c r="DY2" s="6">
+        <v>8.4202085004009622E-2</v>
+      </c>
+      <c r="DZ2" s="6">
+        <v>8.7521001985642277E-2</v>
+      </c>
+      <c r="EA2" s="6">
+        <v>8.6554621848739494E-2</v>
+      </c>
+      <c r="EB2" s="6">
+        <v>8.0152102594691327E-2</v>
+      </c>
+      <c r="EC2" s="6">
+        <v>7.8339645058290636E-2</v>
+      </c>
+      <c r="ED2" s="6">
+        <v>7.5844952186290976E-2</v>
+      </c>
+      <c r="EE2" s="6">
+        <v>7.5027829313543598E-2</v>
+      </c>
+      <c r="EF2" s="6">
+        <v>7.1905609973285836E-2</v>
+      </c>
+      <c r="EG2" s="6">
+        <v>7.3048623226883103E-2</v>
+      </c>
+      <c r="EH2" s="6">
+        <v>7.2435395458104929E-2</v>
+      </c>
+      <c r="EI2" s="6">
+        <v>7.0755433956528349E-2</v>
+      </c>
+      <c r="EJ2" s="6">
+        <v>6.7698259187620888E-2</v>
+      </c>
+      <c r="EK2" s="6">
+        <v>6.4431102650461272E-2</v>
+      </c>
+      <c r="EL2" s="6">
+        <v>6.4513772192591509E-2</v>
+      </c>
+      <c r="EM2" s="6">
+        <v>6.2855454612600642E-2</v>
+      </c>
+      <c r="EN2" s="6">
+        <v>6.0754496271384704E-2</v>
+      </c>
+      <c r="EO2" s="6">
+        <v>6.3898971566848151E-2</v>
+      </c>
+      <c r="EP2" s="6">
+        <v>6.1093484837305395E-2</v>
+      </c>
+      <c r="EQ2" s="6">
+        <v>5.8212209302325582E-2</v>
+      </c>
+      <c r="ER2" s="6">
+        <v>5.6153013352580293E-2</v>
+      </c>
+      <c r="ES2" s="6">
+        <v>6.5025850141993732E-2</v>
+      </c>
+      <c r="ET2" s="6">
+        <v>5.5914768552534903E-2</v>
+      </c>
+      <c r="EU2" s="6">
+        <v>5.1428137344272255E-2</v>
+      </c>
+      <c r="EV2" s="6">
+        <v>6.0331140848264915E-2</v>
+      </c>
+      <c r="EW2" s="6">
+        <v>5.8259029771799913E-2</v>
+      </c>
+      <c r="EX2" s="6">
+        <v>5.8248077066686582E-2</v>
+      </c>
+      <c r="EY2" s="6">
+        <v>5.4601048340128133E-2</v>
+      </c>
+      <c r="EZ2" s="6">
+        <v>5.5060187249219794E-2</v>
+      </c>
+      <c r="FA2" s="6">
+        <v>5.6709086849743247E-2</v>
+      </c>
+      <c r="FB2" s="6">
+        <v>5.7858634059051596E-2</v>
+      </c>
+      <c r="FC2" s="6">
+        <v>5.5726624108148708E-2</v>
+      </c>
+      <c r="FD2" s="6">
+        <v>5.2783386212864145E-2</v>
+      </c>
+      <c r="FE2" s="6">
+        <v>5.3703703703703705E-2</v>
+      </c>
+      <c r="FF2" s="6">
+        <v>5.3008998875140607E-2</v>
+      </c>
+      <c r="FG2" s="6">
+        <v>5.1326937889503536E-2</v>
+      </c>
+      <c r="FH2" s="6">
+        <v>5.328998515796169E-2</v>
+      </c>
+      <c r="FI2" s="6">
+        <v>5.3834543232947604E-2</v>
+      </c>
+      <c r="FJ2" s="6">
+        <v>5.5507621512798387E-2</v>
+      </c>
+      <c r="FK2" s="6">
+        <v>5.5575246331608423E-2</v>
+      </c>
+      <c r="FL2" s="6">
+        <v>5.5138020650417924E-2</v>
+      </c>
+      <c r="FM2" s="6">
+        <v>5.6429620306272292E-2</v>
+      </c>
+      <c r="FN2" s="6">
+        <v>5.6472571468708294E-2</v>
+      </c>
+      <c r="FO2" s="6">
+        <v>5.7207912338124375E-2</v>
+      </c>
+      <c r="FP2" s="6">
+        <v>5.7340266400740796E-2</v>
+      </c>
+      <c r="FQ2" s="6">
+        <v>6.0372977287569844E-2</v>
+      </c>
+      <c r="FR2" s="6">
+        <v>6.2938043173535185E-2</v>
+      </c>
+      <c r="FS2" s="6">
+        <v>5.4288666896314161E-2</v>
+      </c>
+      <c r="FT2" s="6">
+        <v>5.6721109820269254E-2</v>
+      </c>
+      <c r="FU2" s="6">
+        <v>5.7571700373476149E-2</v>
+      </c>
+      <c r="FV2" s="6">
+        <v>5.9160578713651338E-2</v>
+      </c>
+      <c r="FW2" s="6">
+        <v>6.4334836944464985E-2</v>
+      </c>
+      <c r="FX2" s="6">
+        <v>6.2689728203318043E-2</v>
+      </c>
+      <c r="FY2" s="6">
+        <v>6.4052195874842149E-2</v>
+      </c>
+      <c r="FZ2" s="6">
+        <v>6.2338369402477202E-2</v>
+      </c>
+      <c r="GA2" s="6">
+        <v>6.4068914462615256E-2</v>
+      </c>
+      <c r="GB2" s="6">
+        <v>6.6033898305084743E-2</v>
+      </c>
+      <c r="GC2" s="6">
+        <v>6.5638646288209604E-2</v>
+      </c>
+      <c r="GD2" s="6">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="GE2" s="6">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="GF2" s="6">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="GG2" s="6">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="GH2" s="6">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="GI2" s="6">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="GJ2" s="6">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="GK2" s="6">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="GL2" s="6">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="GM2" s="6">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="GN2" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="GO2" s="6">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="GP2" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="GQ2" s="6">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="GR2" s="6">
+        <v>9.9199999999999997E-2</v>
+      </c>
+      <c r="GS2" s="6">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="GT2" s="6">
+        <v>0.1046</v>
+      </c>
+      <c r="GU2" s="6">
+        <v>9.98E-2</v>
+      </c>
+      <c r="GV2" s="6">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="GW2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="GX2" s="6">
+        <v>0.1033</v>
+      </c>
+      <c r="GY2" s="6">
+        <v>0.1062</v>
+      </c>
+      <c r="GZ2" s="6">
+        <v>0.1085</v>
+      </c>
+      <c r="HA2" s="6">
+        <v>0.10730000000000001</v>
+      </c>
+      <c r="HB2" s="6">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="HC2" s="6">
+        <v>0.1009</v>
+      </c>
+      <c r="HD2" s="6">
+        <v>0.1028</v>
+      </c>
+      <c r="HE2" s="6">
+        <v>0.10290000000000001</v>
+      </c>
+      <c r="HF2" s="6">
+        <v>0.1089</v>
+      </c>
+      <c r="HG2" s="6">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="HH2" s="6">
+        <v>0.1197</v>
+      </c>
+      <c r="HI2" s="6">
+        <v>0.11749999999999999</v>
+      </c>
+      <c r="HJ2" s="6">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="HK2" s="6">
+        <v>0.1225</v>
+      </c>
+      <c r="HL2" s="6">
+        <v>0.1295</v>
+      </c>
+      <c r="HM2" s="6">
+        <v>0.13418910457107075</v>
+      </c>
+      <c r="HN2" s="6">
+        <v>0.1366</v>
+      </c>
+      <c r="HO2" s="6">
+        <v>0.1396</v>
+      </c>
+      <c r="HP2" s="6">
+        <v>0.1323</v>
+      </c>
+      <c r="HQ2" s="6">
+        <v>0.1358</v>
+      </c>
+      <c r="HR2" s="6">
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="HS2" s="6">
+        <v>0.1381</v>
+      </c>
+      <c r="HT2" s="6">
+        <v>0.1341</v>
+      </c>
+      <c r="HU2" s="6">
+        <v>0.14349999999999999</v>
+      </c>
+      <c r="HV2" s="6">
+        <v>0.14949999999999999</v>
+      </c>
+      <c r="HW2" s="6">
+        <v>0.1487</v>
+      </c>
+      <c r="HX2" s="6">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="HY2" s="6">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="HZ2" s="6">
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="IA2" s="6">
+        <v>0.1613</v>
+      </c>
+      <c r="IB2" s="6">
+        <v>0.1643</v>
+      </c>
+      <c r="IC2" s="6">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="ID2" s="6">
+        <v>0.15559999999999999</v>
+      </c>
+      <c r="IE2" s="6">
+        <v>0.1515</v>
+      </c>
+      <c r="IF2" s="6">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="IG2" s="6">
+        <v>0.1482</v>
+      </c>
+      <c r="IH2" s="6">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="II2" s="6">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="IJ2" s="6">
+        <v>0.1588</v>
+      </c>
+      <c r="IK2" s="6">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="IL2" s="6">
+        <v>0.1593</v>
+      </c>
+      <c r="IM2" s="6">
+        <v>0.1545</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>